<commit_message>
Updates to all files after debug
</commit_message>
<xml_diff>
--- a/Reference data/Standardized Blynk VPs.xlsx
+++ b/Reference data/Standardized Blynk VPs.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Train_8-16-23-VSC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jpbar\Documents\Arduino\Train_8-16-23-VSC\Reference data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{46E62F32-C700-43A5-AAD5-017DDAA81FD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{930422CE-67FE-4DE4-B108-B0A7934FF164}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{8B86BE9B-45BE-4C57-8E44-34C8A33DD81D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="215">
   <si>
     <t>Light switch</t>
   </si>
@@ -672,6 +672,15 @@
   </si>
   <si>
     <t>Air Pump</t>
+  </si>
+  <si>
+    <t>Train Ready Signal</t>
+  </si>
+  <si>
+    <t>Station 5</t>
+  </si>
+  <si>
+    <t>Station 6</t>
   </si>
 </sst>
 </file>
@@ -739,13 +748,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="distributed"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1062,8 +1071,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E381DDD-8BB5-4C7E-856F-8F973241131A}">
   <dimension ref="A1:K118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="D97" sqref="D97"/>
+    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
+      <selection activeCell="N87" sqref="M87:N87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1321,21 +1330,24 @@
         <v>9</v>
       </c>
     </row>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B39" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D39" s="11" t="s">
+        <v>213</v>
+      </c>
+    </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B40" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>29</v>
+        <v>52</v>
+      </c>
+      <c r="D40" s="11" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B41" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>29</v>
-      </c>
+      <c r="D41" s="11"/>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B42" s="5" t="s">
@@ -1405,8 +1417,8 @@
       <c r="B50" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="D50" s="2" t="s">
-        <v>29</v>
+      <c r="D50" s="11" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.45">
@@ -1428,10 +1440,10 @@
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A56" s="3"/>
-      <c r="H56" s="10" t="s">
+      <c r="H56" s="9" t="s">
         <v>170</v>
       </c>
-      <c r="I56" s="10" t="s">
+      <c r="I56" s="9" t="s">
         <v>171</v>
       </c>
     </row>
@@ -1439,7 +1451,7 @@
       <c r="B57" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="D57" s="9" t="s">
+      <c r="D57" t="s">
         <v>166</v>
       </c>
       <c r="F57" s="4" t="s">
@@ -1556,7 +1568,7 @@
       <c r="B63" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="D63" s="9" t="s">
+      <c r="D63" t="s">
         <v>97</v>
       </c>
       <c r="F63" s="4" t="s">
@@ -1923,10 +1935,10 @@
     <row r="85" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A85" s="3"/>
       <c r="F85" s="3"/>
-      <c r="H85" s="10" t="s">
+      <c r="H85" s="9" t="s">
         <v>170</v>
       </c>
-      <c r="I85" s="10" t="s">
+      <c r="I85" s="9" t="s">
         <v>171</v>
       </c>
     </row>
@@ -2478,7 +2490,7 @@
       <c r="D118" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F118" s="11" t="s">
+      <c r="F118" s="10" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Standardized VPs across all MCUs
</commit_message>
<xml_diff>
--- a/Reference data/Standardized Blynk VPs.xlsx
+++ b/Reference data/Standardized Blynk VPs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jpbar\Documents\Arduino\Train_8-16-23-VSC\Reference data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{930422CE-67FE-4DE4-B108-B0A7934FF164}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42BB96F1-4FDE-4E06-810B-2E6730B941AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{8B86BE9B-45BE-4C57-8E44-34C8A33DD81D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="219">
   <si>
     <t>Light switch</t>
   </si>
@@ -681,6 +681,18 @@
   </si>
   <si>
     <t>Station 6</t>
+  </si>
+  <si>
+    <t>Smoke ON/OFF</t>
+  </si>
+  <si>
+    <t>Park Trigger 1</t>
+  </si>
+  <si>
+    <t>Park Trigger 2</t>
+  </si>
+  <si>
+    <t>Park</t>
   </si>
 </sst>
 </file>
@@ -724,7 +736,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="distributed"/>
@@ -754,7 +766,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1071,8 +1082,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E381DDD-8BB5-4C7E-856F-8F973241131A}">
   <dimension ref="A1:K118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
-      <selection activeCell="N87" sqref="M87:N87"/>
+    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="D65" sqref="D65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1334,7 +1345,7 @@
       <c r="B39" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="D39" s="11" t="s">
+      <c r="D39" t="s">
         <v>213</v>
       </c>
     </row>
@@ -1342,35 +1353,32 @@
       <c r="B40" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="D40" s="11" t="s">
+      <c r="D40" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="D41" s="11"/>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B42" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="D42" s="2" t="s">
-        <v>29</v>
+      <c r="D42" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B43" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="D43" s="2" t="s">
-        <v>29</v>
+      <c r="D43" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="44" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B44" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="D44" s="2" t="s">
-        <v>29</v>
+      <c r="D44" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.45">
@@ -1417,7 +1425,7 @@
       <c r="B50" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="D50" s="11" t="s">
+      <c r="D50" t="s">
         <v>212</v>
       </c>
     </row>
@@ -1552,7 +1560,7 @@
         <v>104</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>29</v>
+        <v>215</v>
       </c>
       <c r="F62" s="4" t="s">
         <v>90</v>
@@ -1562,14 +1570,17 @@
       </c>
       <c r="I62" t="s">
         <v>179</v>
+      </c>
+      <c r="J62" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B63" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="D63" t="s">
-        <v>97</v>
+      <c r="D63" s="2" t="s">
+        <v>29</v>
       </c>
       <c r="F63" s="4" t="s">
         <v>91</v>
@@ -1606,7 +1617,7 @@
         <v>107</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>29</v>
+        <v>97</v>
       </c>
       <c r="F65" s="4" t="s">
         <v>93</v>

</xml_diff>